<commit_message>
made changes for error solving
</commit_message>
<xml_diff>
--- a/dataTemplate/project_import_template.xlsx
+++ b/dataTemplate/project_import_template.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\BusinessComputers.in\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\BusinessComputers.in\Documents\nayashgroup vender management\server\dataTemplate\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="24">
   <si>
     <t>Project Name</t>
   </si>
@@ -27,12 +27,6 @@
     <t>Location</t>
   </si>
   <si>
-    <t>Start Date</t>
-  </si>
-  <si>
-    <t>End Date</t>
-  </si>
-  <si>
     <t>Building Name</t>
   </si>
   <si>
@@ -91,16 +85,29 @@
   </si>
   <si>
     <t>Parking</t>
+  </si>
+  <si>
+    <t>Start Date (yyyy-mm-dd)</t>
+  </si>
+  <si>
+    <t>End Date (yyyy-mm-dd)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -128,7 +135,7 @@
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -434,217 +441,224 @@
   <dimension ref="A1:H8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="4" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.88671875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="F1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="G1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="H1" s="1" t="s">
         <v>5</v>
-      </c>
-      <c r="G1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" t="s">
         <v>8</v>
       </c>
-      <c r="B2" t="s">
+      <c r="D2" t="s">
         <v>9</v>
       </c>
-      <c r="C2" t="s">
+      <c r="E2" t="s">
         <v>10</v>
       </c>
-      <c r="D2" t="s">
+      <c r="F2" t="s">
         <v>11</v>
       </c>
-      <c r="E2" t="s">
+      <c r="G2" t="s">
         <v>12</v>
       </c>
-      <c r="F2" t="s">
+      <c r="H2" t="s">
         <v>13</v>
-      </c>
-      <c r="G2" t="s">
-        <v>14</v>
-      </c>
-      <c r="H2" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" t="s">
         <v>8</v>
       </c>
-      <c r="B3" t="s">
+      <c r="D3" t="s">
         <v>9</v>
       </c>
-      <c r="C3" t="s">
+      <c r="E3" t="s">
         <v>10</v>
       </c>
-      <c r="D3" t="s">
+      <c r="F3" t="s">
         <v>11</v>
       </c>
-      <c r="E3" t="s">
+      <c r="G3" t="s">
         <v>12</v>
       </c>
-      <c r="F3" t="s">
-        <v>13</v>
-      </c>
-      <c r="G3" t="s">
+      <c r="H3" t="s">
         <v>14</v>
-      </c>
-      <c r="H3" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" t="s">
         <v>8</v>
       </c>
-      <c r="B4" t="s">
+      <c r="D4" t="s">
         <v>9</v>
       </c>
-      <c r="C4" t="s">
+      <c r="E4" t="s">
         <v>10</v>
       </c>
-      <c r="D4" t="s">
+      <c r="F4" t="s">
         <v>11</v>
       </c>
-      <c r="E4" t="s">
-        <v>12</v>
-      </c>
-      <c r="F4" t="s">
-        <v>13</v>
-      </c>
       <c r="G4" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="H4" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" t="s">
         <v>8</v>
       </c>
-      <c r="B5" t="s">
+      <c r="D5" t="s">
         <v>9</v>
       </c>
-      <c r="C5" t="s">
+      <c r="E5" t="s">
         <v>10</v>
       </c>
-      <c r="D5" t="s">
-        <v>11</v>
-      </c>
-      <c r="E5" t="s">
+      <c r="F5" t="s">
+        <v>17</v>
+      </c>
+      <c r="G5" t="s">
         <v>12</v>
       </c>
-      <c r="F5" t="s">
-        <v>19</v>
-      </c>
-      <c r="G5" t="s">
-        <v>14</v>
-      </c>
       <c r="H5" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6" t="s">
         <v>8</v>
       </c>
-      <c r="B6" t="s">
+      <c r="D6" t="s">
         <v>9</v>
       </c>
-      <c r="C6" t="s">
+      <c r="E6" t="s">
         <v>10</v>
       </c>
-      <c r="D6" t="s">
-        <v>11</v>
-      </c>
-      <c r="E6" t="s">
+      <c r="F6" t="s">
+        <v>17</v>
+      </c>
+      <c r="G6" t="s">
         <v>12</v>
       </c>
-      <c r="F6" t="s">
+      <c r="H6" t="s">
         <v>19</v>
-      </c>
-      <c r="G6" t="s">
-        <v>14</v>
-      </c>
-      <c r="H6" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>7</v>
+      </c>
+      <c r="C7" t="s">
         <v>8</v>
       </c>
-      <c r="B7" t="s">
+      <c r="D7" t="s">
         <v>9</v>
       </c>
-      <c r="C7" t="s">
-        <v>10</v>
-      </c>
-      <c r="D7" t="s">
+      <c r="E7" t="s">
+        <v>20</v>
+      </c>
+      <c r="F7" t="s">
         <v>11</v>
       </c>
-      <c r="E7" t="s">
-        <v>22</v>
-      </c>
-      <c r="F7" t="s">
-        <v>13</v>
-      </c>
       <c r="G7" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="H7" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" t="s">
+        <v>7</v>
+      </c>
+      <c r="C8" t="s">
         <v>8</v>
       </c>
-      <c r="B8" t="s">
+      <c r="D8" t="s">
         <v>9</v>
       </c>
-      <c r="C8" s="1">
-        <v>45292</v>
-      </c>
-      <c r="D8" s="1">
-        <v>45657</v>
-      </c>
       <c r="E8" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="F8" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
worked on po payment terms and conditions and hrms backend
</commit_message>
<xml_diff>
--- a/dataTemplate/project_import_template.xlsx
+++ b/dataTemplate/project_import_template.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="24">
   <si>
     <t>Project Name</t>
   </si>
@@ -87,16 +87,19 @@
     <t>Parking</t>
   </si>
   <si>
-    <t>Start Date (yyyy-mm-dd)</t>
-  </si>
-  <si>
-    <t>End Date (yyyy-mm-dd)</t>
+    <t>Start Date</t>
+  </si>
+  <si>
+    <t>End Date</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <numFmts count="1">
+    <numFmt numFmtId="165" formatCode="[$-14009]yyyy/mm/dd;@"/>
+  </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -133,9 +136,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -441,14 +450,15 @@
   <dimension ref="A1:H8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
+    <col min="1" max="1" width="21.44140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="8.109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="21" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="20.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.109375" style="3" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="12.6640625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="11.6640625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="14.88671875" bestFit="1" customWidth="1"/>
@@ -462,10 +472,10 @@
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>23</v>
       </c>
       <c r="E1" s="1" t="s">
@@ -488,10 +498,10 @@
       <c r="B2" t="s">
         <v>7</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="3" t="s">
         <v>9</v>
       </c>
       <c r="E2" t="s">
@@ -514,10 +524,10 @@
       <c r="B3" t="s">
         <v>7</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" s="3" t="s">
         <v>9</v>
       </c>
       <c r="E3" t="s">
@@ -540,10 +550,10 @@
       <c r="B4" t="s">
         <v>7</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" s="3" t="s">
         <v>9</v>
       </c>
       <c r="E4" t="s">
@@ -566,10 +576,10 @@
       <c r="B5" t="s">
         <v>7</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D5" s="3" t="s">
         <v>9</v>
       </c>
       <c r="E5" t="s">
@@ -592,10 +602,10 @@
       <c r="B6" t="s">
         <v>7</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D6" s="3" t="s">
         <v>9</v>
       </c>
       <c r="E6" t="s">
@@ -618,10 +628,10 @@
       <c r="B7" t="s">
         <v>7</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="D7" t="s">
+      <c r="D7" s="3" t="s">
         <v>9</v>
       </c>
       <c r="E7" t="s">
@@ -644,10 +654,10 @@
       <c r="B8" t="s">
         <v>7</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C8" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="D8" t="s">
+      <c r="D8" s="3" t="s">
         <v>9</v>
       </c>
       <c r="E8" t="s">
@@ -656,8 +666,19 @@
       <c r="F8" t="s">
         <v>21</v>
       </c>
+      <c r="G8" t="s">
+        <v>15</v>
+      </c>
+      <c r="H8" t="s">
+        <v>21</v>
+      </c>
     </row>
   </sheetData>
+  <dataValidations count="1">
+    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B1:B1048576">
+      <formula1>B3=$B$2</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>